<commit_message>
edit KMK 2 positions, add INterier -center
</commit_message>
<xml_diff>
--- a/КМК с 01.02.xlsx
+++ b/КМК с 01.02.xlsx
@@ -36750,8 +36750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40158,7 +40158,7 @@
         <v>561</v>
       </c>
       <c r="D117" t="s">
-        <v>344</v>
+        <v>581</v>
       </c>
       <c r="F117" t="s">
         <v>1156</v>
@@ -40187,7 +40187,7 @@
         <v>562</v>
       </c>
       <c r="D118" t="s">
-        <v>344</v>
+        <v>581</v>
       </c>
       <c r="F118" t="s">
         <v>1156</v>

</xml_diff>